<commit_message>
updated some data entries
</commit_message>
<xml_diff>
--- a/UUVApplications.xlsx
+++ b/UUVApplications.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Propeller" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="204">
   <si>
     <t xml:space="preserve">Manufacturer</t>
   </si>
@@ -446,6 +446,18 @@
     <t xml:space="preserve">Wichita State University</t>
   </si>
   <si>
+    <t xml:space="preserve">University of Essex iSplah Micro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clapham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Essex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PER</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ho Chi Minh Labriform</t>
   </si>
   <si>
@@ -621,6 +633,9 @@
   </si>
   <si>
     <t xml:space="preserve">Efficient Propulsion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1086,7 @@
   </sheetPr>
   <dimension ref="A1:BC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1929,12 +1944,12 @@
   </sheetPr>
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="bottomRight" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2375,6 +2390,26 @@
       </c>
       <c r="E21" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2447,16 +2482,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>20</v>
@@ -2469,16 +2504,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>20</v>
@@ -2487,16 +2522,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>94</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>20</v>
@@ -2747,16 +2782,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>20</v>
@@ -2765,16 +2800,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>20</v>
@@ -2854,10 +2889,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.83"/>
@@ -2865,15 +2900,15 @@
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>30</v>
@@ -2881,7 +2916,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>59</v>
@@ -2889,15 +2924,15 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>4</v>
@@ -2905,7 +2940,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>34</v>
@@ -2913,7 +2948,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>112</v>
@@ -2921,7 +2956,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>86</v>
@@ -2929,7 +2964,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>25</v>
@@ -2937,7 +2972,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>26</v>
@@ -2945,15 +2980,15 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>47</v>
@@ -2961,7 +2996,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>5</v>
@@ -2969,7 +3004,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>64</v>
@@ -2977,23 +3012,23 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>6</v>
@@ -3001,7 +3036,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>27</v>
@@ -3009,7 +3044,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>18</v>
@@ -3017,7 +3052,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>28</v>
@@ -3025,7 +3060,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>61</v>
@@ -3033,7 +3068,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>22</v>
@@ -3041,7 +3076,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>7</v>
@@ -3049,7 +3084,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>8</v>
@@ -3057,7 +3092,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>48</v>
@@ -3065,7 +3100,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>37</v>
@@ -3073,7 +3108,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>14</v>
@@ -3081,7 +3116,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>37</v>
@@ -3089,7 +3124,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>29</v>
@@ -3097,23 +3132,23 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>20</v>
@@ -3121,15 +3156,15 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>81</v>
@@ -3137,10 +3172,18 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>